<commit_message>
Propuesta modelo de datos
Se ajusta el modelo de datos al flujo de proceso planteado.
</commit_message>
<xml_diff>
--- a/datos/diccionario/DiccionarioDatos.xlsx
+++ b/datos/diccionario/DiccionarioDatos.xlsx
@@ -5,17 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\GitHub\cursoFS\datos\diccionario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\GITHUB\cursoFS\datos\diccionario\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="personas" sheetId="1" r:id="rId1"/>
-    <sheet name="paises" sheetId="4" r:id="rId2"/>
-    <sheet name="actores" sheetId="2" r:id="rId3"/>
-    <sheet name="tipos_identificacion" sheetId="3" r:id="rId4"/>
+    <sheet name="Personas" sheetId="1" r:id="rId1"/>
+    <sheet name="Propuestas" sheetId="6" r:id="rId2"/>
+    <sheet name="Comites" sheetId="7" r:id="rId3"/>
+    <sheet name="Integrantes Comité" sheetId="8" r:id="rId4"/>
+    <sheet name="Registros Propuesta" sheetId="9" r:id="rId5"/>
+    <sheet name="Ejecutores Propuesta" sheetId="10" r:id="rId6"/>
+    <sheet name="Usuarios" sheetId="5" r:id="rId7"/>
+    <sheet name="actores" sheetId="2" r:id="rId8"/>
+    <sheet name="tipos_identificacion" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="106">
   <si>
     <t>Campo</t>
   </si>
@@ -128,22 +133,240 @@
     <t>numero_identificacion</t>
   </si>
   <si>
-    <t>Columna</t>
-  </si>
-  <si>
     <t>Descripción</t>
   </si>
   <si>
-    <t>id_pais</t>
-  </si>
-  <si>
     <t>Numérico</t>
   </si>
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>nombre</t>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>usuario</t>
+  </si>
+  <si>
+    <t>Usuario de sistema</t>
+  </si>
+  <si>
+    <t>Identificador del usuario</t>
+  </si>
+  <si>
+    <t>Contraseña</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Clave de ingreso</t>
+  </si>
+  <si>
+    <t>Fecha de inicio de vigencia</t>
+  </si>
+  <si>
+    <t>Fecha de inicio</t>
+  </si>
+  <si>
+    <t>fecha_inicio</t>
+  </si>
+  <si>
+    <t>Fecha de Fin</t>
+  </si>
+  <si>
+    <t>fecha_fin</t>
+  </si>
+  <si>
+    <t>Fecha de fin de vigencia</t>
+  </si>
+  <si>
+    <t>id_propuesta</t>
+  </si>
+  <si>
+    <t>Identificador de registro</t>
+  </si>
+  <si>
+    <t>Titulo</t>
+  </si>
+  <si>
+    <t>titulo</t>
+  </si>
+  <si>
+    <t>Titulo de la propuesta</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>Descripciòn de la propuesta</t>
+  </si>
+  <si>
+    <t>Postulante</t>
+  </si>
+  <si>
+    <t>id_usuario_postulante</t>
+  </si>
+  <si>
+    <t>Usuario postulante de la propuesta</t>
+  </si>
+  <si>
+    <t>Fecha de postulaciòn</t>
+  </si>
+  <si>
+    <t>fecha_postulacion</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>Estado de la propuesta:
+0: Postulado
+1: Aprobada
+2: Rechazada
+3: En progreso
+4: Finalizada
+5: Suspendida
+6: Cancelado</t>
+  </si>
+  <si>
+    <t>id_comite</t>
+  </si>
+  <si>
+    <t>Propuesta</t>
+  </si>
+  <si>
+    <t>Propuesta estudiada</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>resultado</t>
+  </si>
+  <si>
+    <t>Justificaciòn</t>
+  </si>
+  <si>
+    <t>justificaciòn</t>
+  </si>
+  <si>
+    <t>Justificación del resultado</t>
+  </si>
+  <si>
+    <t>Comité</t>
+  </si>
+  <si>
+    <t>id_comité</t>
+  </si>
+  <si>
+    <t>Participante</t>
+  </si>
+  <si>
+    <t>id_persona_participante</t>
+  </si>
+  <si>
+    <t>Organizador</t>
+  </si>
+  <si>
+    <t>id_persona_organizador</t>
+  </si>
+  <si>
+    <t>Organizador del comité</t>
+  </si>
+  <si>
+    <t>Fecha de creación</t>
+  </si>
+  <si>
+    <t>fecha_creacion</t>
+  </si>
+  <si>
+    <t>Fecha de creación del comité</t>
+  </si>
+  <si>
+    <t>Fecha del comitè</t>
+  </si>
+  <si>
+    <t>Estado del comité:
+0: Planeado
+1: Realizado
+2: Cancelado</t>
+  </si>
+  <si>
+    <t>Asistencia</t>
+  </si>
+  <si>
+    <t>asistencia</t>
+  </si>
+  <si>
+    <t>Asistencia al comité
+0: No
+1: Si</t>
+  </si>
+  <si>
+    <t>Estado de la propuesta:
+1: Aprobada
+2: Rechazada
+4: Finalizada
+5: Suspendida
+6: Cancelada</t>
+  </si>
+  <si>
+    <t>Compromiso</t>
+  </si>
+  <si>
+    <t>compromiso</t>
+  </si>
+  <si>
+    <t>Compromisos del integrantes</t>
+  </si>
+  <si>
+    <t>Propuesta asociada</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Fecha y hora del registro</t>
+  </si>
+  <si>
+    <t>descripcion_registro</t>
+  </si>
+  <si>
+    <t>Descripciòn del registro</t>
+  </si>
+  <si>
+    <t>Persona</t>
+  </si>
+  <si>
+    <t>id_persona_registro</t>
+  </si>
+  <si>
+    <t>Persona que hace el registro</t>
+  </si>
+  <si>
+    <t>Identificador de la propuesta</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>rol</t>
+  </si>
+  <si>
+    <t>Fecha de ejecuciòn</t>
+  </si>
+  <si>
+    <t>fecha_ejecucion</t>
+  </si>
+  <si>
+    <t>Descripciòn de la ejecuciòn</t>
   </si>
 </sst>
 </file>
@@ -181,7 +404,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -220,11 +443,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -232,11 +473,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -250,8 +543,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E9" totalsRowShown="0">
-  <autoFilter ref="A1:E9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E11" totalsRowShown="0">
+  <autoFilter ref="A1:E11"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Columna1"/>
     <tableColumn id="2" name="Campo"/>
@@ -264,14 +557,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E3" totalsRowShown="0">
-  <autoFilter ref="A1:E3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="A1:E5" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:E5"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Columna"/>
+    <tableColumn id="1" name="Columna1"/>
     <tableColumn id="2" name="Campo"/>
     <tableColumn id="3" name="Tipo"/>
     <tableColumn id="4" name="Tamaño"/>
-    <tableColumn id="5" name="Descripción"/>
+    <tableColumn id="5" name="Descripciòn"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -540,11 +833,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -708,6 +999,23 @@
         <v>31</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -718,70 +1026,773 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="13">
+        <v>100</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="13">
+        <v>5000</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="13">
+        <v>200</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="13">
+        <v>5000</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>5000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>5000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>34</v>
+      <c r="E1" s="9" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -792,106 +1803,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5">
-        <v>100</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -954,6 +1868,103 @@
         <v>100</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5">
+        <v>100</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>